<commit_message>
stability parser. add full user when activate token. refactor
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -38,28 +38,64 @@
     <t xml:space="preserve">svvoylov@edu.hse.ru</t>
   </si>
   <si>
-    <t xml:space="preserve">Войлов Сергей Валерьевич</t>
+    <t xml:space="preserve">Сережа</t>
   </si>
   <si>
     <t xml:space="preserve">+79057342253</t>
   </si>
   <si>
-    <t xml:space="preserve">svvoylov@edu.hse.ru1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Войлов Сергей2 Валерьевич</t>
+    <t xml:space="preserve">askonstantinov@miem.hse.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Леша</t>
   </si>
   <si>
     <t xml:space="preserve">+79057342254</t>
   </si>
   <si>
-    <t xml:space="preserve">svvoylov@edu.hse.ru2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Войлов Сергей3 Валерьевич</t>
-  </si>
-  <si>
-    <t xml:space="preserve">+79057342255</t>
+    <t xml:space="preserve">asshadrunov@miem.hse.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Леша Шадрунов</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+790573422551</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maisakov@miem.hse.ru </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Миша</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+790573422552</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vanemna@miem.hse.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Лера</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+790573422543</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amzayakina@miem.hse.ru </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Настя</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+790573422554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dkorolev@miem.hse.ru</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Денис Александрович</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+790573422555</t>
   </si>
   <si>
     <t xml:space="preserve">Название</t>
@@ -83,40 +119,31 @@
     <t xml:space="preserve">Питон</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-02-21 11:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-22 12:00:00</t>
+    <t xml:space="preserve">2022-03-09 20:15:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-09 20:16:00</t>
   </si>
   <si>
     <t xml:space="preserve">МИЭМ</t>
   </si>
   <si>
-    <t xml:space="preserve">Шарага</t>
+    <t xml:space="preserve">Таллинская, д.34</t>
   </si>
   <si>
     <t xml:space="preserve">Плюсы</t>
   </si>
   <si>
-    <t xml:space="preserve">svvoylov@edu.hse.ru;svvoylov@edu.hse.ru2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-21 12:00:00</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2022-02-21 13:00:00</t>
+    <t xml:space="preserve">asshadrunov@miem.hse.ru;svvoylov@edu.hse.ru </t>
   </si>
   <si>
     <t xml:space="preserve">Минуса</t>
   </si>
   <si>
-    <t xml:space="preserve">2022-02-21 13:30:00</t>
-  </si>
-  <si>
     <t xml:space="preserve">ФКН</t>
   </si>
   <si>
-    <t xml:space="preserve">Шарага ещё хуже</t>
+    <t xml:space="preserve">Покровский бул., 11, кор.S</t>
   </si>
 </sst>
 </file>
@@ -127,7 +154,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -167,6 +194,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -212,7 +246,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -237,12 +271,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -262,15 +304,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="40.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.08"/>
   </cols>
   <sheetData>
@@ -288,7 +331,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -299,10 +342,10 @@
         <v>6</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -316,8 +359,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -327,14 +370,69 @@
         <v>12</v>
       </c>
       <c r="D4" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="5" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="5" t="n">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" display="svvoylov@edu.hse.ru"/>
-    <hyperlink ref="A3" r:id="rId2" display="svvoylov@edu.hse.ru1"/>
-    <hyperlink ref="A4" r:id="rId3" display="svvoylov@edu.hse.ru2"/>
+    <hyperlink ref="A3" r:id="rId2" display="askonstantinov@miem.hse.ru"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -354,103 +452,106 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
+      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="37.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="42.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>16</v>
+        <v>28</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="G1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>23</v>
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="G2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>23</v>
+        <v>36</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="G3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>31</v>
+      <c r="C4" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>40</v>
       </c>
       <c r="G4" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="svvoylov@edu.hse.ru"/>
-    <hyperlink ref="B4" r:id="rId2" display="svvoylov@edu.hse.ru1"/>
+    <hyperlink ref="B4" r:id="rId2" display="askonstantinov@miem.hse.ru"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
added re-login for user with /stop. Also add stop, menu, help commands
</commit_message>
<xml_diff>
--- a/sample.xlsx
+++ b/sample.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="42">
   <si>
     <t xml:space="preserve">Email</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t xml:space="preserve">Минуса</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022-03-09 20:30:00</t>
   </si>
   <si>
     <t xml:space="preserve">ФКН</t>
@@ -307,7 +310,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -452,7 +455,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -535,16 +538,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="G4" s="5"/>
     </row>

</xml_diff>